<commit_message>
feat: task #9 To-Do-List push final
</commit_message>
<xml_diff>
--- a/MatrizActividades.xlsx
+++ b/MatrizActividades.xlsx
@@ -431,7 +431,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>20</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,7 +559,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6">
         <f>SUM(C2:C12)</f>
-        <v>345</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>